<commit_message>
Ajout exercice4.bonus et env
</commit_message>
<xml_diff>
--- a/exercices/exercice4/pays_europe.xlsx
+++ b/exercices/exercice4/pays_europe.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="population" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +457,11 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>langue</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>densite</t>
         </is>
       </c>
@@ -477,7 +483,12 @@
       <c r="D2" t="n">
         <v>301336</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>{'ita': 'Italian', 'cat': 'Catalan'}</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
         <v>195.5545736320917</v>
       </c>
     </row>
@@ -498,7 +509,12 @@
       <c r="D3" t="n">
         <v>116</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>{'eng': 'English', 'fra': 'French', 'nrf': 'Jèrriais'}</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
         <v>890.2327586206897</v>
       </c>
     </row>
@@ -519,7 +535,12 @@
       <c r="D4" t="n">
         <v>25713</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>{'mkd': 'Macedonian'}</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
         <v>70.88289970054058</v>
       </c>
     </row>
@@ -540,7 +561,12 @@
       <c r="D5" t="n">
         <v>64559</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>{'lav': 'Latvian'}</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
         <v>28.33067426694961</v>
       </c>
     </row>
@@ -561,7 +587,12 @@
       <c r="D6" t="n">
         <v>45227</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>{'est': 'Estonian'}</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
         <v>30.29152939615716</v>
       </c>
     </row>
@@ -582,7 +613,12 @@
       <c r="D7" t="n">
         <v>207600</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>{'bel': 'Belarusian', 'rus': 'Russian'}</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
         <v>43.87899807321773</v>
       </c>
     </row>
@@ -603,7 +639,12 @@
       <c r="D8" t="n">
         <v>41284</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>{'fra': 'French', 'gsw': 'Swiss German', 'ita': 'Italian', 'roh': 'Romansh'}</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
         <v>220.0089138649356</v>
       </c>
     </row>
@@ -624,7 +665,12 @@
       <c r="D9" t="n">
         <v>10908</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>{'sqi': 'Albanian', 'srp': 'Serbian'}</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
         <v>145.3580858085809</v>
       </c>
     </row>
@@ -645,7 +691,12 @@
       <c r="D10" t="n">
         <v>160</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>{'deu': 'German'}</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
         <v>255.625</v>
       </c>
     </row>
@@ -666,7 +717,12 @@
       <c r="D11" t="n">
         <v>30528</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>{'deu': 'German', 'fra': 'French', 'nld': 'Dutch'}</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
         <v>387.3673676624738</v>
       </c>
     </row>
@@ -687,7 +743,12 @@
       <c r="D12" t="n">
         <v>103000</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>{'isl': 'Icelandic'}</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
         <v>3.803980582524272</v>
       </c>
     </row>
@@ -708,7 +769,12 @@
       <c r="D13" t="n">
         <v>20273</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>{'slv': 'Slovene'}</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
         <v>105.0973215606965</v>
       </c>
     </row>
@@ -729,7 +795,12 @@
       <c r="D14" t="n">
         <v>1580</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>{'swe': 'Swedish'}</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
         <v>19.40126582278481</v>
       </c>
     </row>
@@ -750,7 +821,12 @@
       <c r="D15" t="n">
         <v>603550</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>{'ukr': 'Ukrainian'}</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
         <v>54.44785021953442</v>
       </c>
     </row>
@@ -771,7 +847,12 @@
       <c r="D16" t="n">
         <v>78</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>{'eng': 'English', 'fra': 'French', 'nfr': 'Guernésiais'}</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
         <v>830.525641025641</v>
       </c>
     </row>
@@ -792,7 +873,12 @@
       <c r="D17" t="n">
         <v>78865</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>{'ces': 'Czech', 'slk': 'Slovak'}</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
         <v>137.9869523869904</v>
       </c>
     </row>
@@ -813,7 +899,12 @@
       <c r="D18" t="n">
         <v>0.49</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>{'ita': 'Italian', 'lat': 'Latin'}</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
         <v>1800</v>
       </c>
     </row>
@@ -834,7 +925,12 @@
       <c r="D19" t="n">
         <v>13812</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>{'cnr': 'Montenegrin'}</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
         <v>45.12938024905879</v>
       </c>
     </row>
@@ -855,7 +951,12 @@
       <c r="D20" t="n">
         <v>83871</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>{'deu': 'German'}</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
         <v>109.7033658833208</v>
       </c>
     </row>
@@ -876,7 +977,12 @@
       <c r="D21" t="n">
         <v>312679</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>{'pol': 'Polish'}</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
         <v>119.585901195795</v>
       </c>
     </row>
@@ -897,7 +1003,12 @@
       <c r="D22" t="n">
         <v>2.02</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>{'fra': 'French'}</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
         <v>19021.28712871287</v>
       </c>
     </row>
@@ -918,7 +1029,12 @@
       <c r="D23" t="n">
         <v>49037</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>{'slk': 'Slovak'}</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
         <v>110.4026143524278</v>
       </c>
     </row>
@@ -939,7 +1055,12 @@
       <c r="D24" t="n">
         <v>65300</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>{'lit': 'Lithuanian'}</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
         <v>44.33209800918836</v>
       </c>
     </row>
@@ -960,7 +1081,12 @@
       <c r="D25" t="n">
         <v>543908</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>{'fra': 'French'}</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
         <v>121.9911437228355</v>
       </c>
     </row>
@@ -981,7 +1107,12 @@
       <c r="D26" t="n">
         <v>505992</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>{'spa': 'Spanish', 'cat': 'Catalan', 'eus': 'Basque', 'glc': 'Galician'}</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
         <v>97.46389073345033</v>
       </c>
     </row>
@@ -1002,7 +1133,12 @@
       <c r="D27" t="n">
         <v>386224</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>{'nno': 'Norwegian Nynorsk', 'nob': 'Norwegian Bokmål', 'smi': 'Sami'}</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
         <v>14.51733708935747</v>
       </c>
     </row>
@@ -1023,7 +1159,12 @@
       <c r="D28" t="n">
         <v>70273</v>
       </c>
-      <c r="E28" t="n">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>{'eng': 'English', 'gle': 'Irish'}</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
         <v>77.6770594680745</v>
       </c>
     </row>
@@ -1044,7 +1185,12 @@
       <c r="D29" t="n">
         <v>338455</v>
       </c>
-      <c r="E29" t="n">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>{'fin': 'Finnish', 'swe': 'Swedish'}</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
         <v>16.69446455215612</v>
       </c>
     </row>
@@ -1065,7 +1211,12 @@
       <c r="D30" t="n">
         <v>357114</v>
       </c>
-      <c r="E30" t="n">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>{'deu': 'German'}</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
         <v>233.7943877865332</v>
       </c>
     </row>
@@ -1086,7 +1237,12 @@
       <c r="D31" t="n">
         <v>6</v>
       </c>
-      <c r="E31" t="n">
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>{'eng': 'English'}</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
         <v>6333.333333333333</v>
       </c>
     </row>
@@ -1107,7 +1263,12 @@
       <c r="D32" t="n">
         <v>244376</v>
       </c>
-      <c r="E32" t="n">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>{'eng': 'English'}</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
         <v>283.5034414181425</v>
       </c>
     </row>
@@ -1128,7 +1289,12 @@
       <c r="D33" t="n">
         <v>450295</v>
       </c>
-      <c r="E33" t="n">
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>{'swe': 'Swedish'}</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
         <v>23.551445163726</v>
       </c>
     </row>
@@ -1149,7 +1315,12 @@
       <c r="D34" t="n">
         <v>1393</v>
       </c>
-      <c r="E34" t="n">
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>{'dan': 'Danish', 'fao': 'Faroese'}</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
         <v>39.40057430007179</v>
       </c>
     </row>
@@ -1170,7 +1341,12 @@
       <c r="D35" t="n">
         <v>572</v>
       </c>
-      <c r="E35" t="n">
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>{'eng': 'English', 'glv': 'Manx'}</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
         <v>147.7797202797203</v>
       </c>
     </row>
@@ -1191,7 +1367,12 @@
       <c r="D36" t="n">
         <v>43094</v>
       </c>
-      <c r="E36" t="n">
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>{'dan': 'Danish'}</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
         <v>139.4970993641806</v>
       </c>
     </row>
@@ -1212,7 +1393,12 @@
       <c r="D37" t="n">
         <v>316</v>
       </c>
-      <c r="E37" t="n">
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>{'eng': 'English', 'mlt': 'Maltese'}</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
         <v>1817.246835443038</v>
       </c>
     </row>
@@ -1233,7 +1419,12 @@
       <c r="D38" t="n">
         <v>33847</v>
       </c>
-      <c r="E38" t="n">
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>{'ron': 'Romanian'}</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
         <v>81.22066948326292</v>
       </c>
     </row>
@@ -1254,7 +1445,12 @@
       <c r="D39" t="n">
         <v>468</v>
       </c>
-      <c r="E39" t="n">
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>{'cat': 'Catalan'}</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
         <v>188.9017094017094</v>
       </c>
     </row>
@@ -1275,7 +1471,12 @@
       <c r="D40" t="n">
         <v>131990</v>
       </c>
-      <c r="E40" t="n">
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>{'ell': 'Greek'}</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
         <v>78.7993029774983</v>
       </c>
     </row>
@@ -1296,7 +1497,12 @@
       <c r="D41" t="n">
         <v>56594</v>
       </c>
-      <c r="E41" t="n">
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>{'hrv': 'Croatian'}</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
         <v>68.31524543237799</v>
       </c>
     </row>
@@ -1317,7 +1523,12 @@
       <c r="D42" t="n">
         <v>61</v>
       </c>
-      <c r="E42" t="n">
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>{'ita': 'Italian'}</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
         <v>559.5409836065573</v>
       </c>
     </row>
@@ -1338,7 +1549,12 @@
       <c r="D43" t="n">
         <v>41865</v>
       </c>
-      <c r="E43" t="n">
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>{'nld': 'Dutch'}</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
         <v>432.3524662605996</v>
       </c>
     </row>
@@ -1359,7 +1575,12 @@
       <c r="D44" t="n">
         <v>110879</v>
       </c>
-      <c r="E44" t="n">
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>{'bul': 'Bulgarian'}</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
         <v>58.05752216380018</v>
       </c>
     </row>
@@ -1380,7 +1601,12 @@
       <c r="D45" t="n">
         <v>61399</v>
       </c>
-      <c r="E45" t="n">
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>{'nor': 'Norwegian'}</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
         <v>0.04120588283196795</v>
       </c>
     </row>
@@ -1401,7 +1627,12 @@
       <c r="D46" t="n">
         <v>2586</v>
       </c>
-      <c r="E46" t="n">
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>{'deu': 'German', 'fra': 'French', 'ltz': 'Luxembourgish'}</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
         <v>263.7173240525909</v>
       </c>
     </row>
@@ -1422,7 +1653,12 @@
       <c r="D47" t="n">
         <v>17098246</v>
       </c>
-      <c r="E47" t="n">
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>{'rus': 'Russian'}</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
         <v>8.540544158740024</v>
       </c>
     </row>
@@ -1443,7 +1679,12 @@
       <c r="D48" t="n">
         <v>92090</v>
       </c>
-      <c r="E48" t="n">
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>{'por': 'Portuguese'}</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
         <v>116.7296666304702</v>
       </c>
     </row>
@@ -1464,7 +1705,12 @@
       <c r="D49" t="n">
         <v>93028</v>
       </c>
-      <c r="E49" t="n">
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>{'hun': 'Hungarian'}</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
         <v>102.5444167347465</v>
       </c>
     </row>
@@ -1485,7 +1731,12 @@
       <c r="D50" t="n">
         <v>238391</v>
       </c>
-      <c r="E50" t="n">
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>{'ron': 'Romanian'}</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
         <v>79.8521378743325</v>
       </c>
     </row>
@@ -1506,7 +1757,12 @@
       <c r="D51" t="n">
         <v>28748</v>
       </c>
-      <c r="E51" t="n">
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>{'sqi': 'Albanian'}</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
         <v>82.20794490051482</v>
       </c>
     </row>
@@ -1527,7 +1783,12 @@
       <c r="D52" t="n">
         <v>51209</v>
       </c>
-      <c r="E52" t="n">
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>{'bos': 'Bosnian', 'hrv': 'Croatian', 'srp': 'Serbian'}</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
         <v>66.82419106016521</v>
       </c>
     </row>
@@ -1548,7 +1809,12 @@
       <c r="D53" t="n">
         <v>77589</v>
       </c>
-      <c r="E53" t="n">
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>{'srp': 'Serbian'}</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
         <v>84.64837799172562</v>
       </c>
     </row>
@@ -1569,8 +1835,88 @@
       <c r="D54" t="n">
         <v>9251</v>
       </c>
-      <c r="E54" t="n">
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>{'ell': 'Greek', 'tur': 'Turkish'}</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
         <v>155.9414117392714</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>langue</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>nb_pays</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>population_totale</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>rus</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>155137605</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>cat</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>108331988</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>deu</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>105240604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>